<commit_message>
updated ontological definitions: academic publications & events
</commit_message>
<xml_diff>
--- a/docs/OntologyDataset_Mapping.xlsx
+++ b/docs/OntologyDataset_Mapping.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spitxa/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDCD449-8806-ED48-97DA-8AD6A34CFEA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C8C3DB-3953-3845-88A8-A87467861D86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ontología" sheetId="8" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Project" sheetId="1" r:id="rId3"/>
     <sheet name="Document" sheetId="11" r:id="rId4"/>
     <sheet name="Agent" sheetId="12" r:id="rId5"/>
+    <sheet name="Event" sheetId="13" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Agent!$A$3:$F$40</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="601">
   <si>
     <t>APP</t>
   </si>
@@ -1252,9 +1253,6 @@
   </si>
   <si>
     <t>app.DedicacionInvestigador</t>
-  </si>
-  <si>
-    <t>EQUIPO INVESTIGADOR (Person)</t>
   </si>
   <si>
     <t>PROYECTO (Project)</t>
@@ -1435,9 +1433,6 @@
     <t>Un proyecto está coordinado por</t>
   </si>
   <si>
-    <t>Un proyecto tiene una sescripción visual</t>
-  </si>
-  <si>
     <t>Un proyecto es competitivo o no</t>
   </si>
   <si>
@@ -1513,9 +1508,6 @@
     <t>Un libro tiene un dominio científico</t>
   </si>
   <si>
-    <t>Un libro tiene un publicador</t>
-  </si>
-  <si>
     <t>Un libro tiene citas</t>
   </si>
   <si>
@@ -1781,6 +1773,93 @@
   </si>
   <si>
     <t>Una persona es contratada por un agente (grupo, organización)</t>
+  </si>
+  <si>
+    <t>Un proyecto tiene una descripción visual</t>
+  </si>
+  <si>
+    <t>TESIS EXTERNA  (Document &gt; Publication &gt; Academic Publication &gt; Thesis&gt;Bachelor/Master/PHD)</t>
+  </si>
+  <si>
+    <t>TESINA EXTERNA  (Document &gt; Publication &gt; Academic Publication &gt; Thesis&gt;Bachelor/Master/PHD)</t>
+  </si>
+  <si>
+    <t>PERSONA (Person)</t>
+  </si>
+  <si>
+    <t>CONGRESO (Event Series &gt; Conference/Workshop)</t>
+  </si>
+  <si>
+    <t>Temporalentity time</t>
+  </si>
+  <si>
+    <t>Agent agent</t>
+  </si>
+  <si>
+    <t>Spatialthing place</t>
+  </si>
+  <si>
+    <t>Event subevent</t>
+  </si>
+  <si>
+    <t>Person coadvisedby</t>
+  </si>
+  <si>
+    <t>Academicdegree requiredfor</t>
+  </si>
+  <si>
+    <t>tesiPremio</t>
+  </si>
+  <si>
+    <t>No hay Autor</t>
+  </si>
+  <si>
+    <t>lugarCelebracion</t>
+  </si>
+  <si>
+    <t>fechaCelebracion</t>
+  </si>
+  <si>
+    <t>congNumero</t>
+  </si>
+  <si>
+    <t>Una publicación académica tiene un dominio científico</t>
+  </si>
+  <si>
+    <t>Una publicación académica tiene un coautor</t>
+  </si>
+  <si>
+    <t>Una publicación académica cita a otra publicación académica</t>
+  </si>
+  <si>
+    <t>Un libro es publicado por</t>
+  </si>
+  <si>
+    <t>Una publicación académica está publicada por</t>
+  </si>
+  <si>
+    <t>Una publicación académica há sido premiada/galardonada con_ por_</t>
+  </si>
+  <si>
+    <t>Una publicación académica há sido dirigida por_</t>
+  </si>
+  <si>
+    <t>Una publicación académica es obligatoria para obtener un grado académico</t>
+  </si>
+  <si>
+    <t>Una publicación académica tiene código DOI</t>
+  </si>
+  <si>
+    <t>Una publicación académica tiene un número de citas</t>
+  </si>
+  <si>
+    <t>Un congreso tiene una localización física (se celebra en un lugar)</t>
+  </si>
+  <si>
+    <t>Un congreso tiene una fecha y un horario</t>
+  </si>
+  <si>
+    <t>Un congreso tiene una persona como autor que contribuye</t>
   </si>
 </sst>
 </file>
@@ -2028,7 +2107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2114,6 +2193,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2168,12 +2250,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2184,6 +2260,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2210,7 +2292,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2508,7 +2590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H79"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
@@ -2523,35 +2605,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="48" t="s">
         <v>335</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="H2" s="39" t="s">
-        <v>417</v>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="H2" s="40" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>416</v>
-      </c>
       <c r="G3" s="6"/>
-      <c r="H3" s="40"/>
+      <c r="H3" s="41"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="16" t="s">
@@ -2586,10 +2668,10 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="46" t="s">
         <v>260</v>
       </c>
       <c r="D7" s="18" t="s">
@@ -2600,8 +2682,8 @@
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="44"/>
-      <c r="C8" s="45"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="18" t="s">
         <v>261</v>
       </c>
@@ -2610,20 +2692,20 @@
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="18" t="s">
         <v>185</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="32"/>
       <c r="H9" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="46"/>
       <c r="D10" s="18" t="s">
         <v>293</v>
       </c>
@@ -2632,12 +2714,12 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="46" t="s">
+      <c r="B11" s="45"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="47" t="s">
         <v>294</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="49" t="s">
         <v>205</v>
       </c>
       <c r="F11" s="32" t="s">
@@ -2648,10 +2730,10 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="44"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="48"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="49"/>
       <c r="F12" s="32" t="s">
         <v>300</v>
       </c>
@@ -2660,10 +2742,10 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="44"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="48"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="49"/>
       <c r="F13" s="32" t="s">
         <v>298</v>
       </c>
@@ -2672,8 +2754,8 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="44"/>
-      <c r="C14" s="45"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="46"/>
       <c r="D14" s="18" t="s">
         <v>248</v>
       </c>
@@ -2682,8 +2764,8 @@
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="44"/>
-      <c r="C15" s="45"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="46"/>
       <c r="D15" s="18" t="s">
         <v>245</v>
       </c>
@@ -2692,8 +2774,8 @@
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="20" t="s">
         <v>295</v>
       </c>
@@ -2702,9 +2784,9 @@
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="46" t="s">
+      <c r="B17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="47" t="s">
         <v>296</v>
       </c>
       <c r="E17" s="21" t="s">
@@ -2718,9 +2800,9 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="44"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="46"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="47"/>
       <c r="E18" s="19" t="s">
         <v>301</v>
       </c>
@@ -2728,9 +2810,9 @@
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="44"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="46"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="47"/>
       <c r="E19" s="19" t="s">
         <v>302</v>
       </c>
@@ -2740,9 +2822,9 @@
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="46"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="47"/>
       <c r="E20" s="19" t="s">
         <v>303</v>
       </c>
@@ -2752,21 +2834,21 @@
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="46"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="47"/>
       <c r="E21" s="19" t="s">
         <v>183</v>
       </c>
       <c r="F21" s="32"/>
       <c r="H21" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="44"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="46"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="47"/>
       <c r="E22" s="19" t="s">
         <v>304</v>
       </c>
@@ -2774,9 +2856,9 @@
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="44"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="46"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="47"/>
       <c r="E23" s="19" t="s">
         <v>255</v>
       </c>
@@ -2784,7 +2866,7 @@
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="44"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="22" t="s">
         <v>291</v>
       </c>
@@ -2828,7 +2910,7 @@
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="42" t="s">
         <v>246</v>
       </c>
       <c r="C28" s="24" t="s">
@@ -2840,11 +2922,11 @@
       <c r="E28" s="21"/>
       <c r="F28" s="33"/>
       <c r="H28" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="42"/>
+      <c r="B29" s="43"/>
       <c r="C29" s="27" t="s">
         <v>256</v>
       </c>
@@ -2856,11 +2938,11 @@
       </c>
       <c r="F29" s="34"/>
       <c r="H29" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="42"/>
+      <c r="B30" s="43"/>
       <c r="C30" s="27"/>
       <c r="D30" s="30"/>
       <c r="E30" s="21" t="s">
@@ -2870,7 +2952,7 @@
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="42"/>
+      <c r="B31" s="43"/>
       <c r="C31" s="27"/>
       <c r="D31" s="30"/>
       <c r="E31" s="21" t="s">
@@ -2880,7 +2962,7 @@
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="42"/>
+      <c r="B32" s="43"/>
       <c r="C32" s="27"/>
       <c r="D32" s="25" t="s">
         <v>310</v>
@@ -2892,7 +2974,7 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B33" s="42"/>
+      <c r="B33" s="43"/>
       <c r="C33" s="27"/>
       <c r="D33" s="25" t="s">
         <v>311</v>
@@ -2902,7 +2984,7 @@
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" s="42"/>
+      <c r="B34" s="43"/>
       <c r="C34" s="31"/>
       <c r="D34" s="25" t="s">
         <v>265</v>
@@ -2914,7 +2996,7 @@
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B35" s="43"/>
+      <c r="B35" s="44"/>
       <c r="C35" s="24" t="s">
         <v>186</v>
       </c>
@@ -2922,11 +3004,11 @@
       <c r="E35" s="21"/>
       <c r="F35" s="33"/>
       <c r="H35" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="42" t="s">
         <v>271</v>
       </c>
       <c r="C36" s="24" t="s">
@@ -2938,7 +3020,7 @@
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B37" s="42"/>
+      <c r="B37" s="43"/>
       <c r="C37" s="24" t="s">
         <v>314</v>
       </c>
@@ -2948,7 +3030,7 @@
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="43"/>
+      <c r="B38" s="44"/>
       <c r="C38" s="24" t="s">
         <v>315</v>
       </c>
@@ -3050,7 +3132,7 @@
       <c r="H47" s="5"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B48" s="41" t="s">
+      <c r="B48" s="42" t="s">
         <v>280</v>
       </c>
       <c r="C48" s="24" t="s">
@@ -3066,7 +3148,7 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B49" s="42"/>
+      <c r="B49" s="43"/>
       <c r="C49" s="24" t="s">
         <v>318</v>
       </c>
@@ -3076,7 +3158,7 @@
       <c r="H49" s="5"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="42"/>
+      <c r="B50" s="43"/>
       <c r="C50" s="24" t="s">
         <v>319</v>
       </c>
@@ -3086,7 +3168,7 @@
       <c r="H50" s="5"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B51" s="43"/>
+      <c r="B51" s="44"/>
       <c r="C51" s="24" t="s">
         <v>320</v>
       </c>
@@ -3106,7 +3188,7 @@
       <c r="H52" s="5"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="42" t="s">
         <v>321</v>
       </c>
       <c r="C53" s="24" t="s">
@@ -3118,12 +3200,12 @@
       <c r="E53" s="21"/>
       <c r="F53" s="33"/>
       <c r="H53" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B54" s="42"/>
-      <c r="C54" s="37" t="s">
+      <c r="B54" s="43"/>
+      <c r="C54" s="38" t="s">
         <v>247</v>
       </c>
       <c r="D54" s="25" t="s">
@@ -3134,8 +3216,8 @@
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="42"/>
-      <c r="C55" s="38"/>
+      <c r="B55" s="43"/>
+      <c r="C55" s="39"/>
       <c r="D55" s="25" t="s">
         <v>325</v>
       </c>
@@ -3144,7 +3226,7 @@
       <c r="H55" s="5"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="42"/>
+      <c r="B56" s="43"/>
       <c r="C56" s="24" t="s">
         <v>253</v>
       </c>
@@ -3158,7 +3240,7 @@
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="43"/>
+      <c r="B57" s="44"/>
       <c r="C57" s="24" t="s">
         <v>322</v>
       </c>
@@ -3178,7 +3260,7 @@
       <c r="H58" s="5"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="42" t="s">
         <v>328</v>
       </c>
       <c r="C59" s="24" t="s">
@@ -3190,7 +3272,7 @@
       <c r="H59" s="5"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B60" s="43"/>
+      <c r="B60" s="44"/>
       <c r="C60" s="24" t="s">
         <v>327</v>
       </c>
@@ -3200,7 +3282,7 @@
       <c r="H60" s="5"/>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B61" s="41" t="s">
+      <c r="B61" s="42" t="s">
         <v>182</v>
       </c>
       <c r="C61" s="24" t="s">
@@ -3214,7 +3296,7 @@
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="42"/>
+      <c r="B62" s="43"/>
       <c r="C62" s="24" t="s">
         <v>331</v>
       </c>
@@ -3226,7 +3308,7 @@
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B63" s="42"/>
+      <c r="B63" s="43"/>
       <c r="C63" s="24" t="s">
         <v>332</v>
       </c>
@@ -3238,7 +3320,7 @@
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B64" s="42"/>
+      <c r="B64" s="43"/>
       <c r="C64" s="24" t="s">
         <v>333</v>
       </c>
@@ -3250,7 +3332,7 @@
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B65" s="43"/>
+      <c r="B65" s="44"/>
       <c r="C65" s="24" t="s">
         <v>334</v>
       </c>
@@ -3334,7 +3416,7 @@
       <c r="H72" s="5"/>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B73" s="41" t="s">
+      <c r="B73" s="42" t="s">
         <v>286</v>
       </c>
       <c r="C73" s="24" t="s">
@@ -3346,7 +3428,7 @@
       <c r="H73" s="5"/>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B74" s="43"/>
+      <c r="B74" s="44"/>
       <c r="C74" s="24" t="s">
         <v>206</v>
       </c>
@@ -3453,18 +3535,18 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="E2" s="47" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2" s="48" t="s">
         <v>335</v>
       </c>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
@@ -3472,19 +3554,19 @@
       </c>
       <c r="C3" s="5"/>
       <c r="E3" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>412</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>413</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>414</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>415</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
@@ -3537,10 +3619,10 @@
       <c r="C7" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="F7" s="46" t="s">
         <v>260</v>
       </c>
       <c r="G7" s="18" t="s">
@@ -3556,8 +3638,8 @@
       <c r="C8" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="E8" s="44"/>
-      <c r="F8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="46"/>
       <c r="G8" s="18" t="s">
         <v>261</v>
       </c>
@@ -3571,8 +3653,8 @@
       <c r="C9" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="46"/>
       <c r="G9" s="18" t="s">
         <v>185</v>
       </c>
@@ -3586,8 +3668,8 @@
       <c r="C10" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="E10" s="44"/>
-      <c r="F10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="46"/>
       <c r="G10" s="18" t="s">
         <v>293</v>
       </c>
@@ -3601,12 +3683,12 @@
       <c r="C11" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="46" t="s">
+      <c r="E11" s="45"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="47" t="s">
         <v>294</v>
       </c>
-      <c r="H11" s="48" t="s">
+      <c r="H11" s="49" t="s">
         <v>205</v>
       </c>
       <c r="I11" s="32" t="s">
@@ -3620,10 +3702,10 @@
       <c r="C12" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="E12" s="44"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="48"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="49"/>
       <c r="I12" s="32" t="s">
         <v>300</v>
       </c>
@@ -3635,10 +3717,10 @@
       <c r="C13" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="E13" s="44"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="48"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="49"/>
       <c r="I13" s="32" t="s">
         <v>298</v>
       </c>
@@ -3650,8 +3732,8 @@
       <c r="C14" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="E14" s="44"/>
-      <c r="F14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="46"/>
       <c r="G14" s="18" t="s">
         <v>248</v>
       </c>
@@ -3665,8 +3747,8 @@
       <c r="C15" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="E15" s="44"/>
-      <c r="F15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="46"/>
       <c r="G15" s="18" t="s">
         <v>245</v>
       </c>
@@ -3680,8 +3762,8 @@
       <c r="C16" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="E16" s="44"/>
-      <c r="F16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="46"/>
       <c r="G16" s="20" t="s">
         <v>295</v>
       </c>
@@ -3693,9 +3775,9 @@
         <v>55</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="46" t="s">
+      <c r="E17" s="45"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="47" t="s">
         <v>296</v>
       </c>
       <c r="H17" s="21" t="s">
@@ -3710,9 +3792,9 @@
         <v>56</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="46"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="47"/>
       <c r="H18" s="19" t="s">
         <v>301</v>
       </c>
@@ -3725,9 +3807,9 @@
       <c r="C19" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="E19" s="44"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="46"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="47"/>
       <c r="H19" s="19" t="s">
         <v>302</v>
       </c>
@@ -3742,9 +3824,9 @@
       <c r="C20" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="E20" s="44"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="46"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="47"/>
       <c r="H20" s="19" t="s">
         <v>303</v>
       </c>
@@ -3757,9 +3839,9 @@
         <v>59</v>
       </c>
       <c r="C21" s="5"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="46"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="47"/>
       <c r="H21" s="19" t="s">
         <v>183</v>
       </c>
@@ -3772,9 +3854,9 @@
       <c r="C22" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="E22" s="44"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="46"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="47"/>
       <c r="H22" s="19" t="s">
         <v>304</v>
       </c>
@@ -3785,9 +3867,9 @@
         <v>61</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="46"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="47"/>
       <c r="H23" s="19" t="s">
         <v>255</v>
       </c>
@@ -3800,7 +3882,7 @@
       <c r="C24" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="E24" s="44"/>
+      <c r="E24" s="45"/>
       <c r="F24" s="22" t="s">
         <v>291</v>
       </c>
@@ -3858,7 +3940,7 @@
         <v>66</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="E28" s="41" t="s">
+      <c r="E28" s="42" t="s">
         <v>246</v>
       </c>
       <c r="F28" s="24" t="s">
@@ -3875,7 +3957,7 @@
         <v>67</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="E29" s="42"/>
+      <c r="E29" s="43"/>
       <c r="F29" s="27" t="s">
         <v>256</v>
       </c>
@@ -3894,7 +3976,7 @@
       <c r="C30" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="E30" s="42"/>
+      <c r="E30" s="43"/>
       <c r="F30" s="27"/>
       <c r="G30" s="30"/>
       <c r="H30" s="21" t="s">
@@ -3909,7 +3991,7 @@
       <c r="C31" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="E31" s="42"/>
+      <c r="E31" s="43"/>
       <c r="F31" s="27"/>
       <c r="G31" s="30"/>
       <c r="H31" s="21" t="s">
@@ -3924,7 +4006,7 @@
       <c r="C32" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="E32" s="42"/>
+      <c r="E32" s="43"/>
       <c r="F32" s="27"/>
       <c r="G32" s="25" t="s">
         <v>310</v>
@@ -3937,7 +4019,7 @@
         <v>71</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="E33" s="42"/>
+      <c r="E33" s="43"/>
       <c r="F33" s="27"/>
       <c r="G33" s="25" t="s">
         <v>311</v>
@@ -3950,7 +4032,7 @@
         <v>72</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="E34" s="42"/>
+      <c r="E34" s="43"/>
       <c r="F34" s="31"/>
       <c r="G34" s="25" t="s">
         <v>265</v>
@@ -3967,7 +4049,7 @@
       <c r="C35" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="E35" s="43"/>
+      <c r="E35" s="44"/>
       <c r="F35" s="24" t="s">
         <v>186</v>
       </c>
@@ -3982,7 +4064,7 @@
       <c r="C36" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="E36" s="41" t="s">
+      <c r="E36" s="42" t="s">
         <v>271</v>
       </c>
       <c r="F36" s="24" t="s">
@@ -3999,7 +4081,7 @@
       <c r="C37" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="E37" s="42"/>
+      <c r="E37" s="43"/>
       <c r="F37" s="24" t="s">
         <v>314</v>
       </c>
@@ -4012,7 +4094,7 @@
         <v>76</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="E38" s="43"/>
+      <c r="E38" s="44"/>
       <c r="F38" s="24" t="s">
         <v>315</v>
       </c>
@@ -4148,7 +4230,7 @@
         <v>86</v>
       </c>
       <c r="C48" s="5"/>
-      <c r="E48" s="41" t="s">
+      <c r="E48" s="42" t="s">
         <v>280</v>
       </c>
       <c r="F48" s="24" t="s">
@@ -4167,7 +4249,7 @@
       <c r="C49" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="E49" s="42"/>
+      <c r="E49" s="43"/>
       <c r="F49" s="24" t="s">
         <v>318</v>
       </c>
@@ -4182,7 +4264,7 @@
       <c r="C50" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="E50" s="42"/>
+      <c r="E50" s="43"/>
       <c r="F50" s="24" t="s">
         <v>319</v>
       </c>
@@ -4197,7 +4279,7 @@
       <c r="C51" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="E51" s="43"/>
+      <c r="E51" s="44"/>
       <c r="F51" s="24" t="s">
         <v>320</v>
       </c>
@@ -4225,7 +4307,7 @@
         <v>91</v>
       </c>
       <c r="C53" s="5"/>
-      <c r="E53" s="41" t="s">
+      <c r="E53" s="42" t="s">
         <v>321</v>
       </c>
       <c r="F53" s="24" t="s">
@@ -4244,8 +4326,8 @@
       <c r="C54" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="E54" s="42"/>
-      <c r="F54" s="37" t="s">
+      <c r="E54" s="43"/>
+      <c r="F54" s="38" t="s">
         <v>247</v>
       </c>
       <c r="G54" s="25" t="s">
@@ -4261,8 +4343,8 @@
       <c r="C55" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="E55" s="42"/>
-      <c r="F55" s="38"/>
+      <c r="E55" s="43"/>
+      <c r="F55" s="39"/>
       <c r="G55" s="25" t="s">
         <v>325</v>
       </c>
@@ -4274,7 +4356,7 @@
         <v>94</v>
       </c>
       <c r="C56" s="5"/>
-      <c r="E56" s="42"/>
+      <c r="E56" s="43"/>
       <c r="F56" s="24" t="s">
         <v>253</v>
       </c>
@@ -4289,7 +4371,7 @@
         <v>95</v>
       </c>
       <c r="C57" s="5"/>
-      <c r="E57" s="43"/>
+      <c r="E57" s="44"/>
       <c r="F57" s="24" t="s">
         <v>322</v>
       </c>
@@ -4345,7 +4427,7 @@
       <c r="C61" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="E61" s="41" t="s">
+      <c r="E61" s="42" t="s">
         <v>182</v>
       </c>
       <c r="F61" s="24" t="s">
@@ -4362,7 +4444,7 @@
       <c r="C62" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="E62" s="42"/>
+      <c r="E62" s="43"/>
       <c r="F62" s="24" t="s">
         <v>331</v>
       </c>
@@ -4377,7 +4459,7 @@
       <c r="C63" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="E63" s="42"/>
+      <c r="E63" s="43"/>
       <c r="F63" s="24" t="s">
         <v>332</v>
       </c>
@@ -4392,7 +4474,7 @@
       <c r="C64" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E64" s="42"/>
+      <c r="E64" s="43"/>
       <c r="F64" s="24" t="s">
         <v>333</v>
       </c>
@@ -4407,7 +4489,7 @@
       <c r="C65" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E65" s="43"/>
+      <c r="E65" s="44"/>
       <c r="F65" s="24" t="s">
         <v>334</v>
       </c>
@@ -4523,7 +4605,7 @@
         <v>110</v>
       </c>
       <c r="C73" s="5"/>
-      <c r="E73" s="41" t="s">
+      <c r="E73" s="42" t="s">
         <v>286</v>
       </c>
       <c r="F73" s="24" t="s">
@@ -4540,7 +4622,7 @@
       <c r="C74" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="E74" s="43"/>
+      <c r="E74" s="44"/>
       <c r="F74" s="24" t="s">
         <v>206</v>
       </c>
@@ -5117,8 +5199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5127,33 +5209,33 @@
     <col min="2" max="3" width="30.6640625" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
     <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="126.6640625" customWidth="1"/>
+    <col min="6" max="6" width="156.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
-        <v>407</v>
-      </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="53"/>
+      <c r="A1" s="52" t="s">
+        <v>406</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="54"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="39" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="39" t="s">
-        <v>447</v>
-      </c>
-      <c r="F2" s="54" t="s">
+      <c r="E2" s="40" t="s">
+        <v>446</v>
+      </c>
+      <c r="F2" s="55" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5167,9 +5249,9 @@
       <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -5179,10 +5261,10 @@
         <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -5193,10 +5275,10 @@
         <v>2</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -5211,7 +5293,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F6" s="5"/>
     </row>
@@ -5227,7 +5309,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -5239,10 +5321,10 @@
         <v>5</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -5253,10 +5335,10 @@
         <v>6</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -5271,10 +5353,10 @@
         <v>7</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -5289,7 +5371,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F11" s="5"/>
     </row>
@@ -5305,7 +5387,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F12" s="5"/>
     </row>
@@ -5317,15 +5399,15 @@
         <v>10</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
@@ -5335,10 +5417,10 @@
         <v>11</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -5349,10 +5431,10 @@
         <v>12</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>459</v>
+        <v>572</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -5363,10 +5445,10 @@
         <v>13</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -5377,10 +5459,10 @@
         <v>14</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -5389,16 +5471,16 @@
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -5413,7 +5495,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F19" s="5"/>
     </row>
@@ -5425,10 +5507,10 @@
         <v>17</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -5439,10 +5521,10 @@
         <v>18</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -5453,10 +5535,10 @@
         <v>19</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -5467,10 +5549,10 @@
         <v>20</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -5496,10 +5578,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5507,34 +5589,34 @@
     <col min="1" max="1" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.6640625" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="125.5" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="60" t="s">
-        <v>409</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
+      <c r="A1" s="59" t="s">
+        <v>408</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="54" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="54" t="s">
-        <v>447</v>
-      </c>
-      <c r="F2" s="54" t="s">
+      <c r="E2" s="55" t="s">
+        <v>446</v>
+      </c>
+      <c r="F2" s="55" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5548,9 +5630,9 @@
       <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
@@ -5564,10 +5646,10 @@
         <v>187</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -5582,7 +5664,7 @@
         <v>188</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>194</v>
@@ -5600,7 +5682,7 @@
         <v>189</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>194</v>
@@ -5618,10 +5700,10 @@
         <v>190</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -5632,7 +5714,7 @@
         <v>191</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F8" s="5"/>
     </row>
@@ -5644,7 +5726,7 @@
         <v>192</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F9" s="5"/>
     </row>
@@ -5656,23 +5738,23 @@
         <v>193</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="55" t="s">
+      <c r="A11" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="39" t="s">
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="39" t="s">
-        <v>447</v>
-      </c>
-      <c r="F11" s="39" t="s">
+      <c r="E11" s="40" t="s">
+        <v>446</v>
+      </c>
+      <c r="F11" s="40" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5686,9 +5768,9 @@
       <c r="C12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
@@ -5698,7 +5780,7 @@
         <v>187</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F13" s="5"/>
     </row>
@@ -5716,10 +5798,10 @@
         <v>188</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -5736,7 +5818,7 @@
         <v>189</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>194</v>
@@ -5754,7 +5836,7 @@
         <v>190</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F16" s="5"/>
     </row>
@@ -5766,7 +5848,7 @@
         <v>191</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F17" s="5"/>
     </row>
@@ -5778,7 +5860,7 @@
         <v>192</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F18" s="5"/>
     </row>
@@ -5796,33 +5878,33 @@
         <v>193</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F19" s="11"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="57" t="s">
-        <v>410</v>
-      </c>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="59"/>
+      <c r="A21" s="56" t="s">
+        <v>409</v>
+      </c>
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="58"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="39" t="s">
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="39" t="s">
-        <v>447</v>
-      </c>
-      <c r="F22" s="54" t="s">
+      <c r="E22" s="40" t="s">
+        <v>446</v>
+      </c>
+      <c r="F22" s="55" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5836,9 +5918,9 @@
       <c r="C23" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="54"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="54"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="55"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
@@ -5848,7 +5930,7 @@
         <v>339</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="F24" s="5"/>
     </row>
@@ -5864,7 +5946,7 @@
         <v>191</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F25" s="5"/>
     </row>
@@ -5882,7 +5964,7 @@
         <v>340</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>194</v>
@@ -5902,7 +5984,7 @@
         <v>341</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F27" s="5"/>
     </row>
@@ -5914,7 +5996,7 @@
         <v>342</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F28" s="5"/>
     </row>
@@ -5926,7 +6008,7 @@
         <v>343</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F29" s="5"/>
     </row>
@@ -5938,7 +6020,7 @@
         <v>344</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="F30" s="10"/>
     </row>
@@ -5954,7 +6036,7 @@
         <v>365</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F31" s="10"/>
     </row>
@@ -5970,7 +6052,7 @@
         <v>366</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F32" s="10"/>
     </row>
@@ -5983,28 +6065,28 @@
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="57" t="s">
-        <v>419</v>
-      </c>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="59"/>
+      <c r="A34" s="56" t="s">
+        <v>418</v>
+      </c>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="58"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="49" t="s">
+      <c r="A35" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="39" t="s">
+      <c r="B35" s="51"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="39" t="s">
-        <v>447</v>
-      </c>
-      <c r="F35" s="54" t="s">
+      <c r="E35" s="40" t="s">
+        <v>446</v>
+      </c>
+      <c r="F35" s="55" t="s">
         <v>36</v>
       </c>
     </row>
@@ -6018,9 +6100,9 @@
       <c r="C36" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="54"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="54"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="55"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
@@ -6030,7 +6112,7 @@
         <v>339</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="F37" s="5"/>
     </row>
@@ -6042,16 +6124,16 @@
         <v>191</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>35</v>
@@ -6060,7 +6142,7 @@
         <v>340</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>485</v>
+        <v>591</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>194</v>
@@ -6068,22 +6150,22 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="C40" s="8" t="s">
         <v>421</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>423</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>422</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>341</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -6094,7 +6176,7 @@
         <v>342</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="F41" s="5"/>
     </row>
@@ -6106,7 +6188,7 @@
         <v>343</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="F42" s="5"/>
     </row>
@@ -6118,13 +6200,13 @@
         <v>344</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="F43" s="10"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8" t="s">
@@ -6134,7 +6216,7 @@
         <v>365</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="F44" s="10"/>
     </row>
@@ -6146,14 +6228,318 @@
         <v>366</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="F45" s="10"/>
     </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="56" t="s">
+        <v>573</v>
+      </c>
+      <c r="B47" s="57"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="58"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="51"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" s="40" t="s">
+        <v>446</v>
+      </c>
+      <c r="F48" s="55" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C49" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" s="55"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="55"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="8"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8" t="s">
+        <v>583</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="F56" s="10"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="F57" s="10"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="F58" s="10"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="56" t="s">
+        <v>574</v>
+      </c>
+      <c r="B60" s="57"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="57"/>
+      <c r="E60" s="57"/>
+      <c r="F60" s="58"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="51"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E61" s="40" t="s">
+        <v>446</v>
+      </c>
+      <c r="F61" s="55" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C62" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D62" s="55"/>
+      <c r="E62" s="41"/>
+      <c r="F62" s="55"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="8"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="8"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="8"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="8"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="8"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="F69" s="10"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="8"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="F70" s="10"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="8"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="F71" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E22:E23"/>
+  <mergeCells count="29">
     <mergeCell ref="E35:E36"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="D35:D36"/>
@@ -6171,6 +6557,18 @@
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="A34:F34"/>
     <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="A60:F60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="F61:F62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6181,8 +6579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45:E114"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6190,34 +6588,34 @@
     <col min="1" max="1" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.6640625" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="62.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41.1640625" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="59"/>
+      <c r="A1" s="56" t="s">
+        <v>410</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="58"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="39" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="39" t="s">
-        <v>447</v>
-      </c>
-      <c r="F2" s="54" t="s">
+      <c r="E2" s="40" t="s">
+        <v>446</v>
+      </c>
+      <c r="F2" s="55" t="s">
         <v>36</v>
       </c>
     </row>
@@ -6231,9 +6629,9 @@
       <c r="C3" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="54"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="55"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -6243,16 +6641,16 @@
         <v>244</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>226</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -6263,7 +6661,7 @@
         <v>243</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="F5" s="5"/>
     </row>
@@ -6275,7 +6673,7 @@
         <v>238</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F6" s="5"/>
     </row>
@@ -6287,7 +6685,7 @@
         <v>212</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -6299,7 +6697,7 @@
         <v>221</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="F8" s="5"/>
     </row>
@@ -6311,7 +6709,7 @@
         <v>217</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F9" s="5"/>
     </row>
@@ -6323,7 +6721,7 @@
         <v>224</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="F10" s="10"/>
     </row>
@@ -6335,7 +6733,7 @@
         <v>222</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="F11" s="5"/>
     </row>
@@ -6347,7 +6745,7 @@
         <v>219</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="F12" s="5"/>
     </row>
@@ -6359,7 +6757,7 @@
         <v>241</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="F13" s="5"/>
     </row>
@@ -6371,7 +6769,7 @@
         <v>232</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F14" s="5"/>
     </row>
@@ -6383,7 +6781,7 @@
         <v>209</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F15" s="5"/>
     </row>
@@ -6395,7 +6793,7 @@
         <v>220</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="F16" s="5"/>
     </row>
@@ -6407,7 +6805,7 @@
         <v>239</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F17" s="5"/>
     </row>
@@ -6419,7 +6817,7 @@
         <v>233</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="F18" s="5"/>
     </row>
@@ -6431,7 +6829,7 @@
         <v>225</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F19" s="5"/>
     </row>
@@ -6443,13 +6841,13 @@
         <v>218</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>197</v>
@@ -6461,7 +6859,7 @@
         <v>228</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>194</v>
@@ -6469,7 +6867,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>197</v>
@@ -6481,7 +6879,7 @@
         <v>211</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>194</v>
@@ -6489,7 +6887,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>197</v>
@@ -6501,7 +6899,7 @@
         <v>215</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>194</v>
@@ -6521,7 +6919,7 @@
         <v>223</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>361</v>
@@ -6541,7 +6939,7 @@
         <v>230</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>361</v>
@@ -6555,7 +6953,7 @@
         <v>236</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F26" s="5"/>
     </row>
@@ -6567,7 +6965,7 @@
         <v>242</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="F27" s="5"/>
     </row>
@@ -6579,7 +6977,7 @@
         <v>214</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="F28" s="5"/>
     </row>
@@ -6591,7 +6989,7 @@
         <v>207</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="F29" s="5"/>
     </row>
@@ -6603,7 +7001,7 @@
         <v>234</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F30" s="5"/>
     </row>
@@ -6615,7 +7013,7 @@
         <v>213</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F31" s="5"/>
     </row>
@@ -6627,7 +7025,7 @@
         <v>210</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F32" s="5"/>
     </row>
@@ -6645,7 +7043,7 @@
         <v>235</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F33" s="5"/>
     </row>
@@ -6657,7 +7055,7 @@
         <v>216</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F34" s="5"/>
     </row>
@@ -6669,7 +7067,7 @@
         <v>227</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F35" s="5"/>
     </row>
@@ -6687,7 +7085,7 @@
         <v>231</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="F36" s="5"/>
     </row>
@@ -6699,7 +7097,7 @@
         <v>240</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="F37" s="5"/>
     </row>
@@ -6711,7 +7109,7 @@
         <v>237</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="F38" s="5"/>
     </row>
@@ -6723,7 +7121,7 @@
         <v>229</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="F39" s="5"/>
     </row>
@@ -6735,33 +7133,33 @@
         <v>208</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="F40" s="5"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="51" t="s">
-        <v>406</v>
-      </c>
-      <c r="B42" s="52"/>
-      <c r="C42" s="52"/>
-      <c r="D42" s="52"/>
-      <c r="E42" s="52"/>
-      <c r="F42" s="53"/>
+      <c r="A42" s="52" t="s">
+        <v>575</v>
+      </c>
+      <c r="B42" s="53"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="54"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="50"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="39" t="s">
+      <c r="B43" s="51"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="39" t="s">
-        <v>447</v>
-      </c>
-      <c r="F43" s="54" t="s">
+      <c r="E43" s="40" t="s">
+        <v>446</v>
+      </c>
+      <c r="F43" s="55" t="s">
         <v>36</v>
       </c>
     </row>
@@ -6775,9 +7173,9 @@
       <c r="C44" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D44" s="40"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="41"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
@@ -6791,7 +7189,7 @@
         <v>221</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="F45" s="5"/>
     </row>
@@ -6807,7 +7205,7 @@
         <v>368</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F46" s="5"/>
     </row>
@@ -6823,7 +7221,7 @@
         <v>369</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F47" s="5"/>
     </row>
@@ -6835,7 +7233,7 @@
         <v>370</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F48" s="5"/>
     </row>
@@ -6847,7 +7245,7 @@
         <v>240</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="F49" s="5"/>
     </row>
@@ -6863,7 +7261,7 @@
         <v>212</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="F50" s="5"/>
     </row>
@@ -6875,7 +7273,7 @@
         <v>371</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="F51" s="10"/>
     </row>
@@ -6887,7 +7285,7 @@
         <v>211</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="F52" s="5"/>
     </row>
@@ -6903,7 +7301,7 @@
         <v>372</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="F53" s="5"/>
     </row>
@@ -6915,7 +7313,7 @@
         <v>215</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="F54" s="5"/>
     </row>
@@ -6931,7 +7329,7 @@
         <v>224</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F55" s="5"/>
     </row>
@@ -6947,7 +7345,7 @@
         <v>373</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F56" s="5"/>
     </row>
@@ -6959,7 +7357,7 @@
         <v>374</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="F57" s="5"/>
     </row>
@@ -6975,7 +7373,7 @@
         <v>375</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="F58" s="5"/>
     </row>
@@ -6991,7 +7389,7 @@
         <v>376</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F59" s="5"/>
     </row>
@@ -7003,7 +7401,7 @@
         <v>377</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="F60" s="5"/>
     </row>
@@ -7019,7 +7417,7 @@
         <v>378</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>194</v>
@@ -7033,7 +7431,7 @@
         <v>379</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F62" s="5"/>
     </row>
@@ -7045,7 +7443,7 @@
         <v>380</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="F63" s="5"/>
     </row>
@@ -7061,7 +7459,7 @@
         <v>209</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="F64" s="5"/>
     </row>
@@ -7073,7 +7471,7 @@
         <v>381</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="F65" s="5"/>
     </row>
@@ -7085,7 +7483,7 @@
         <v>228</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="F66" s="5"/>
     </row>
@@ -7097,7 +7495,7 @@
         <v>210</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="F67" s="5"/>
     </row>
@@ -7113,7 +7511,7 @@
         <v>239</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F68" s="5"/>
     </row>
@@ -7129,7 +7527,7 @@
         <v>382</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>194</v>
@@ -7143,7 +7541,7 @@
         <v>383</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="F70" s="5"/>
     </row>
@@ -7155,7 +7553,7 @@
         <v>235</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="F71" s="5"/>
     </row>
@@ -7171,7 +7569,7 @@
         <v>219</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="F72" s="5"/>
     </row>
@@ -7183,7 +7581,7 @@
         <v>214</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="F73" s="5"/>
     </row>
@@ -7195,7 +7593,7 @@
         <v>225</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="F74" s="5"/>
     </row>
@@ -7207,7 +7605,7 @@
         <v>384</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="F75" s="5"/>
     </row>
@@ -7219,7 +7617,7 @@
         <v>242</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="F76" s="5"/>
     </row>
@@ -7235,7 +7633,7 @@
         <v>241</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="F77" s="5"/>
     </row>
@@ -7251,7 +7649,7 @@
         <v>385</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="F78" s="5"/>
     </row>
@@ -7263,7 +7661,7 @@
         <v>216</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F79" s="5"/>
     </row>
@@ -7275,7 +7673,7 @@
         <v>208</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="F80" s="5"/>
     </row>
@@ -7291,7 +7689,7 @@
         <v>217</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="F81" s="5"/>
     </row>
@@ -7303,7 +7701,7 @@
         <v>386</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="F82" s="5"/>
     </row>
@@ -7321,7 +7719,7 @@
         <v>387</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>194</v>
@@ -7335,7 +7733,7 @@
         <v>230</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="F84" s="5"/>
     </row>
@@ -7347,7 +7745,7 @@
         <v>388</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="F85" s="5"/>
     </row>
@@ -7363,7 +7761,7 @@
         <v>389</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F86" s="5"/>
     </row>
@@ -7379,7 +7777,7 @@
         <v>232</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="F87" s="5"/>
     </row>
@@ -7395,7 +7793,7 @@
         <v>222</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F88" s="5"/>
     </row>
@@ -7407,7 +7805,7 @@
         <v>390</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="F89" s="5"/>
     </row>
@@ -7419,7 +7817,7 @@
         <v>236</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="F90" s="5"/>
     </row>
@@ -7431,7 +7829,7 @@
         <v>238</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F91" s="5"/>
     </row>
@@ -7453,7 +7851,7 @@
         <v>391</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="F93" s="5"/>
     </row>
@@ -7465,25 +7863,25 @@
         <v>227</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F94" s="5"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="B95" s="13" t="s">
         <v>432</v>
       </c>
-      <c r="B95" s="13" t="s">
-        <v>433</v>
-      </c>
       <c r="C95" s="13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D95" s="9" t="s">
         <v>226</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="F95" s="5"/>
     </row>
@@ -7495,7 +7893,7 @@
         <v>213</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="F96" s="5"/>
     </row>
@@ -7511,7 +7909,7 @@
         <v>392</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F97" s="5"/>
     </row>
@@ -7523,7 +7921,7 @@
         <v>393</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="F98" s="5"/>
     </row>
@@ -7535,7 +7933,7 @@
         <v>229</v>
       </c>
       <c r="E99" s="9" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="F99" s="5"/>
     </row>
@@ -7547,7 +7945,7 @@
         <v>223</v>
       </c>
       <c r="E100" s="9" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="F100" s="5"/>
     </row>
@@ -7559,7 +7957,7 @@
         <v>234</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F101" s="5"/>
     </row>
@@ -7575,7 +7973,7 @@
         <v>373</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="F102" s="5"/>
     </row>
@@ -7587,7 +7985,7 @@
         <v>394</v>
       </c>
       <c r="E103" s="9" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="F103" s="5"/>
     </row>
@@ -7599,7 +7997,7 @@
         <v>395</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F104" s="5"/>
     </row>
@@ -7611,7 +8009,7 @@
         <v>396</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="F105" s="5"/>
     </row>
@@ -7623,7 +8021,7 @@
         <v>243</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F106" s="5"/>
     </row>
@@ -7635,7 +8033,7 @@
         <v>397</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="F107" s="5"/>
     </row>
@@ -7651,7 +8049,7 @@
         <v>398</v>
       </c>
       <c r="E108" s="9" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="F108" s="5"/>
     </row>
@@ -7663,7 +8061,7 @@
         <v>399</v>
       </c>
       <c r="E109" s="9" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="F109" s="5"/>
     </row>
@@ -7675,7 +8073,7 @@
         <v>400</v>
       </c>
       <c r="E110" s="9" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="F110" s="5"/>
     </row>
@@ -7687,7 +8085,7 @@
         <v>233</v>
       </c>
       <c r="E111" s="9" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="F111" s="5"/>
     </row>
@@ -7699,7 +8097,7 @@
         <v>218</v>
       </c>
       <c r="E112" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F112" s="5"/>
     </row>
@@ -7715,7 +8113,7 @@
         <v>220</v>
       </c>
       <c r="E113" s="9" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="F113" s="5"/>
     </row>
@@ -7727,7 +8125,7 @@
         <v>237</v>
       </c>
       <c r="E114" s="9" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="F114" s="5"/>
     </row>
@@ -7748,4 +8146,230 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6493D9AE-7547-43AE-8437-829B44CAF591}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.1640625" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="11.5" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
+        <v>576</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="58"/>
+    </row>
+    <row r="2" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>446</v>
+      </c>
+      <c r="F2" s="55" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="55"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="55"/>
+    </row>
+    <row r="4" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>586</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>577</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>587</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>600</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>585</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>579</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>598</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9" t="s">
+        <v>580</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>